<commit_message>
Core Data Model and Users ingestion
</commit_message>
<xml_diff>
--- a/IXM eDW - POC/Data Sources.xlsx
+++ b/IXM eDW - POC/Data Sources.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2135f97aab0e4312/999 - Microsoft Cloud/IXM eDW - POC/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bdbelux1-my.sharepoint.com/personal/rfranco_adflux_net/Documents/999 - Microsoft Cloud/IXM eDW - POC/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="9" documentId="8_{F7429AFB-A570-4014-86CE-AFC7524966EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{95FE3B5D-EADC-44F8-ACE5-AB9855B7F4C4}"/>
+  <xr:revisionPtr revIDLastSave="41" documentId="8_{F7429AFB-A570-4014-86CE-AFC7524966EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CDD3B9F9-7C66-4C1C-A653-44D0AF6C41D2}"/>
   <bookViews>
-    <workbookView xWindow="6930" yWindow="1050" windowWidth="15615" windowHeight="13020" xr2:uid="{586EBBDA-C70E-465C-84DC-AB7B81BE5BB1}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{586EBBDA-C70E-465C-84DC-AB7B81BE5BB1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="25">
   <si>
     <t>Contract_Details</t>
   </si>
@@ -93,6 +93,27 @@
   </si>
   <si>
     <t>L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                             + CAST(A.[_application] AS NVARCHAR(MAX)) + '|' 
+                                             + CAST(A.[_username] AS NVARCHAR(MAX)) + '|'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                             + CAST(A.[_strGUID] AS NVARCHAR(MAX)) + '|'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                             + CAST(A.[_Party_ID] AS NVARCHAR(MAX)) + '|' 
+                                             + CAST(A.[_party_code] AS NVARCHAR(MAX)) + '|'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                             + CAST(A.[_AutoID] AS NVARCHAR(MAX)) + '|'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                             + CAST(A.[_UserID] AS NVARCHAR(MAX)) + '|' 
+                                             + CAST(A.[_Username] AS NVARCHAR(MAX)) + '|'</t>
+  </si>
+  <si>
+    <t>_party_code</t>
   </si>
 </sst>
 </file>
@@ -108,12 +129,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -128,8 +155,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -464,133 +503,176 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D48B640-0219-4569-893C-DAD2B01E4747}">
-  <dimension ref="D3:F20"/>
+  <dimension ref="D3:I20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="54.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="38.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="3" width="9.140625" style="1"/>
+    <col min="4" max="4" width="54.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="38.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="9.140625" style="1"/>
+    <col min="8" max="8" width="94.7109375" style="1" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D3" t="s">
+    <row r="3" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D3" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D4" t="s">
+    <row r="4" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D4" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D5" t="s">
+    <row r="5" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D5" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D6" t="s">
+    <row r="6" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D6" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D7" t="s">
+    <row r="7" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D7" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D8" t="s">
+    <row r="8" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D8" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D9" t="s">
+    <row r="9" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D9" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D10" t="s">
+    <row r="10" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D10" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D11" t="s">
+    <row r="11" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D11" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="E12" t="s">
+    <row r="12" spans="4:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="E12" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="E13" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F12" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="13" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="E13" t="s">
+      <c r="F13" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="E14" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="E15" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F13" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="14" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="E14" t="s">
-        <v>11</v>
-      </c>
-      <c r="F14" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="15" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="E15" t="s">
+      <c r="F15" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="E16" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="5:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="E17" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F15" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="16" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="E16" t="s">
+      <c r="F17" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G17" s="3"/>
+      <c r="H17" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E18" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E19" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="F16" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="17" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E17" t="s">
+      <c r="F19" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" spans="5:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="E20" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="F17" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="18" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E18" t="s">
-        <v>15</v>
-      </c>
-      <c r="F18" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="19" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E19" t="s">
-        <v>16</v>
-      </c>
-      <c r="F19" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="20" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E20" t="s">
-        <v>17</v>
-      </c>
-      <c r="F20" t="s">
-        <v>18</v>
+      <c r="F20" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G20" s="3"/>
+      <c r="H20" s="4" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>